<commit_message>
Exclude empty font, border and fill sections in differential styles
# Conflicts:
#	ClosedXML/Excel/XLWorkbook_Save.cs
#	ClosedXML_Tests/Resource/Examples/Misc/AddingDataSet.xlsx
#	ClosedXML_Tests/Resource/Examples/Misc/AddingDataTableAsWorksheet.xlsx
#	ClosedXML_Tests/Resource/Examples/Misc/CopyingWorksheets.xlsx
#	ClosedXML_Tests/Resource/Examples/Misc/ShowCase.xlsx
#	ClosedXML_Tests/Resource/Examples/Ranges/AddingRowToTables.xlsx
#	ClosedXML_Tests/Resource/Examples/Tables/InsertingTables.xlsx
#	ClosedXML_Tests/Resource/Examples/Tables/UsingTables.xlsx
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFDatesOccurring.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFDatesOccurring.xlsx
@@ -74,44 +74,36 @@
   </x:cellStyles>
   <x:dxfs count="4">
     <x:dxf>
-      <x:font/>
       <x:fill>
         <x:patternFill patternType="solid">
           <x:fgColor auto="1"/>
           <x:bgColor rgb="FFA8E4A0"/>
         </x:patternFill>
       </x:fill>
-      <x:border/>
     </x:dxf>
     <x:dxf>
-      <x:font/>
       <x:fill>
         <x:patternFill patternType="solid">
           <x:fgColor auto="1"/>
           <x:bgColor rgb="FFFFA500"/>
         </x:patternFill>
       </x:fill>
-      <x:border/>
     </x:dxf>
     <x:dxf>
-      <x:font/>
       <x:fill>
         <x:patternFill patternType="solid">
           <x:fgColor auto="1"/>
           <x:bgColor rgb="FF0000FF"/>
         </x:patternFill>
       </x:fill>
-      <x:border/>
     </x:dxf>
     <x:dxf>
-      <x:font/>
       <x:fill>
         <x:patternFill patternType="solid">
           <x:fgColor auto="1"/>
           <x:bgColor rgb="FFFF0000"/>
         </x:patternFill>
       </x:fill>
-      <x:border/>
     </x:dxf>
   </x:dxfs>
 </x:styleSheet>

</xml_diff>